<commit_message>
Fixing broken selenium tests --  https://jenkins.tlt.harvard.edu/job/canvas_course_admin_tools_selenium_tests/ws/reports/canvas_course_admin_tools_test_report_20160520_18_38_36.html
- 1 is due to spaces in the locator
- 1 is to due to invalid test data (confirmed with PO "Teaching Staff" is not a dropdown in the Manage People Tool.)
</commit_message>
<xml_diff>
--- a/selenium_tests/manage_people/test_data/mp_test_users_with_roles.xlsx
+++ b/selenium_tests/manage_people/test_data/mp_test_users_with_roles.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ely817/tlt/icommons_lti_tools/selenium_tests/manage_people/test_data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>univ_id</t>
   </si>
@@ -68,9 +63,6 @@
     <t>MP_001_user_email</t>
   </si>
   <si>
-    <t>Teaching Staff</t>
-  </si>
-  <si>
     <t>Observer</t>
   </si>
   <si>
@@ -78,9 +70,6 @@
   </si>
   <si>
     <t>MP_003_user_email</t>
-  </si>
-  <si>
-    <t>MP_004_user_email</t>
   </si>
   <si>
     <t>Teaching Fellow</t>
@@ -690,13 +679,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
@@ -710,7 +699,7 @@
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -742,12 +731,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="17" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4">
         <v>1819036</v>
@@ -774,12 +763,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="17">
       <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1819035</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C3" s="4">
         <v>1819035</v>
@@ -787,83 +776,56 @@
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
+      <c r="E3" s="5">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="b">
-        <v>0</v>
-      </c>
       <c r="J3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="17">
       <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1819036</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1819036</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1819035</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="5">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1819036</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1819036</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="5">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2" display="test54@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="test54@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Updated the test data to reflect the canvas role the test is looking for - Updated the CSS locator due to locator changes that caused existing tests to break - Added some code to better handle sporadic failures due to page not reloading
</commit_message>
<xml_diff>
--- a/selenium_tests/manage_people/test_data/mp_test_users_with_roles.xlsx
+++ b/selenium_tests/manage_people/test_data/mp_test_users_with_roles.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hic048/projects/canvas_manage_course/selenium_tests/manage_people/test_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="17420" yWindow="10040" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>univ_id</t>
   </si>
@@ -75,16 +80,13 @@
     <t>Teaching Fellow</t>
   </si>
   <si>
-    <t>ObserverEnrollment</t>
-  </si>
-  <si>
-    <t>TaEnrollment</t>
-  </si>
-  <si>
     <t>tlttest55@gmail.com</t>
   </si>
   <si>
     <t>tlttest54@gmail.com</t>
+  </si>
+  <si>
+    <t>TA</t>
   </si>
 </sst>
 </file>
@@ -682,24 +684,17 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -731,12 +726,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" customHeight="1">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4">
         <v>1819036</v>
@@ -763,12 +758,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4">
         <v>1819035</v>
@@ -780,7 +775,7 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="b">
         <v>1</v>
@@ -789,7 +784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17">
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -806,7 +801,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>1</v>
@@ -822,10 +817,5 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>